<commit_message>
v1.1 All comments closed as it is not applicaple
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_WF_NAVIGATION_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_WF_NAVIGATION_REVIEWS.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4844BC97-9DF9-44D5-91A5-F04BBEB42A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -106,13 +107,22 @@
   </si>
   <si>
     <t>Initial version</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t>not applicable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All comments closed as it is not applicaple </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +164,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -309,25 +325,25 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -343,16 +359,16 @@
     <xf numFmtId="15" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -634,27 +650,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="54.140625" customWidth="1"/>
-    <col min="6" max="6" width="51.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5546875" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" customWidth="1"/>
+    <col min="5" max="5" width="54.109375" customWidth="1"/>
+    <col min="6" max="6" width="51.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="18.75">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -683,7 +699,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45">
+    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
@@ -706,13 +722,13 @@
         <v>19</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="I2" s="24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="45">
+    <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
@@ -735,13 +751,13 @@
         <v>19</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="I3" s="24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="60">
+    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -764,13 +780,13 @@
         <v>19</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="I4" s="24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -781,7 +797,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -792,7 +808,7 @@
       <c r="H6" s="7"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -803,7 +819,7 @@
       <c r="H7" s="8"/>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -814,7 +830,7 @@
       <c r="H8" s="7"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -825,7 +841,7 @@
       <c r="H9" s="8"/>
       <c r="I9" s="14"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -836,7 +852,7 @@
       <c r="H10" s="7"/>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -847,7 +863,7 @@
       <c r="H11" s="8"/>
       <c r="I11" s="14"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
@@ -860,10 +876,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="I2:I12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="I2:I12" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"open,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="H2:H12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="H2:H12" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -872,22 +888,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="48.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="48.6640625" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25">
+    <row r="1" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
@@ -901,7 +917,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.75">
+    <row r="2" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>13</v>
       </c>
@@ -915,13 +931,22 @@
         <v>45772</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75">
-      <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="20"/>
+    <row r="3" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="20">
+        <v>45772</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v1.2 All reviewer verifications are closed, and the file tab is renamed
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_WF_NAVIGATION_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_WF_NAVIGATION_REVIEWS.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4844BC97-9DF9-44D5-91A5-F04BBEB42A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
+    <sheet name="LH_WF_NAVIGATION_REVIEWS" sheetId="3" r:id="rId1"/>
     <sheet name="VERSION-HISTORY" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -85,9 +84,6 @@
     <t>Omar Sherif</t>
   </si>
   <si>
-    <t>open</t>
-  </si>
-  <si>
     <t>LH_Review_WF_NAVIGATION_002</t>
   </si>
   <si>
@@ -116,13 +112,22 @@
   </si>
   <si>
     <t xml:space="preserve">All comments closed as it is not applicaple </t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>v1.2</t>
+  </si>
+  <si>
+    <t>All reviewer verifications are closed, and the file tab is renamed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -650,27 +655,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5546875" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" customWidth="1"/>
-    <col min="5" max="5" width="54.109375" customWidth="1"/>
-    <col min="6" max="6" width="51.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="54.140625" customWidth="1"/>
+    <col min="6" max="6" width="51.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="18.75">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -699,7 +704,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="45">
       <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
@@ -722,18 +727,18 @@
         <v>19</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="45">
       <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="22" t="s">
         <v>14</v>
@@ -742,27 +747,27 @@
         <v>13</v>
       </c>
       <c r="E3" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="21" t="s">
         <v>22</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>23</v>
       </c>
       <c r="G3" s="22" t="s">
         <v>19</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3" s="24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="60">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>14</v>
@@ -771,22 +776,22 @@
         <v>13</v>
       </c>
       <c r="E4" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="21" t="s">
         <v>24</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>25</v>
       </c>
       <c r="G4" s="22" t="s">
         <v>19</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I4" s="24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="6"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -797,7 +802,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="A6" s="5"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -808,7 +813,7 @@
       <c r="H6" s="7"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7" s="2"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -819,7 +824,7 @@
       <c r="H7" s="8"/>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9">
       <c r="A8" s="5"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -830,7 +835,7 @@
       <c r="H8" s="7"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="A9" s="2"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -841,7 +846,7 @@
       <c r="H9" s="8"/>
       <c r="I9" s="14"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9">
       <c r="A10" s="5"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -852,7 +857,7 @@
       <c r="H10" s="7"/>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11" s="2"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -863,7 +868,7 @@
       <c r="H11" s="8"/>
       <c r="I11" s="14"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9">
       <c r="A12" s="5"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
@@ -876,10 +881,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="I2:I12" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="I2:I12">
       <formula1>"open,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="H2:H12" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="H2:H12">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -888,22 +893,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="48.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="20.25">
       <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
@@ -917,7 +922,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18.75">
       <c r="A2" s="18" t="s">
         <v>13</v>
       </c>
@@ -925,23 +930,37 @@
         <v>14</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="20">
         <v>45772</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="37.5">
       <c r="A3" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="20">
+        <v>45772</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="37.5">
+      <c r="A4" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="20">
         <v>45772</v>
       </c>
     </row>

</xml_diff>